<commit_message>
Upload LB1 and LB2
</commit_message>
<xml_diff>
--- a/LB1/Гистограммы.xlsx
+++ b/LB1/Гистограммы.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -123,16 +123,16 @@
     <t>Подготовительно-заключительная работа</t>
   </si>
   <si>
-    <t>0.95</t>
-  </si>
-  <si>
-    <t>94.3</t>
-  </si>
-  <si>
-    <t>2.4</t>
-  </si>
-  <si>
-    <t>1.43</t>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>82.5</t>
+  </si>
+  <si>
+    <t>2.08</t>
+  </si>
+  <si>
+    <t>1.25</t>
   </si>
 </sst>
 </file>
@@ -266,15 +266,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -291,6 +282,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -412,6 +412,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-A602-44FD-9C86-88824F8A478F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -427,6 +432,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-A602-44FD-9C86-88824F8A478F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -442,6 +452,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-A602-44FD-9C86-88824F8A478F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -457,6 +472,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-A602-44FD-9C86-88824F8A478F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -472,6 +492,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-A602-44FD-9C86-88824F8A478F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -487,6 +512,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-A602-44FD-9C86-88824F8A478F}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -1494,20 +1524,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1545,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1527,7 +1557,7 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1541,7 +1571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1555,7 +1585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1569,7 +1599,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1583,7 +1613,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1597,7 +1627,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1611,7 +1641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +1655,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1639,7 +1669,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1653,7 +1683,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1667,7 +1697,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1681,7 +1711,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1695,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -1709,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
@@ -1717,7 +1747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
@@ -1725,218 +1755,218 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11" t="s">
+      <c r="C21" s="15"/>
+      <c r="D21" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="12" t="s">
+    <row r="22" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="17"/>
+      <c r="B22" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="16"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B23" s="8">
         <v>4</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B24" s="8">
         <v>396</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="8">
         <v>4</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="8">
         <v>10</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
+    <row r="27" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="12" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="8">
         <v>0</v>
       </c>
-      <c r="C27" s="17">
+      <c r="C27" s="14">
         <v>0</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
+    <row r="28" spans="1:4" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="12" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="8">
         <v>6</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>26</v>
       </c>
       <c r="B29" s="8">
-        <v>420</v>
-      </c>
-      <c r="C29" s="17">
+        <v>480</v>
+      </c>
+      <c r="C29" s="14">
         <v>100</v>
       </c>
-      <c r="D29" s="14"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29" s="11"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
     </row>
   </sheetData>

</xml_diff>